<commit_message>
Enhance query_cover_letter function to improve prompt clarity and specificity, refine keyword extraction logic, and update msgbox_similar_application for better user feedback.
</commit_message>
<xml_diff>
--- a/Application History.xlsx
+++ b/Application History.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,11 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Company City</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Original_JD</t>
         </is>
       </c>
     </row>
@@ -540,6 +545,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -614,6 +620,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -692,6 +699,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -770,6 +778,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -846,6 +855,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -926,6 +936,7 @@
           <t>North York</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1006,6 +1017,7 @@
           <t>Calgary</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1084,6 +1096,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1160,6 +1173,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1231,6 +1245,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1309,6 +1324,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1387,6 +1403,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1465,6 +1482,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1543,6 +1561,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1618,6 +1637,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1696,6 +1716,7 @@
           <t>Langley</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1780,6 +1801,7 @@
           <t>Kamloops</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1860,6 +1882,7 @@
           <t>Kamloops</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1944,6 +1967,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2028,6 +2052,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2108,6 +2133,7 @@
           <t>Calgary</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2189,6 +2215,7 @@
           <t>Mississauga</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2273,6 +2300,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2357,6 +2385,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2438,6 +2467,7 @@
           <t>Calgary</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2522,6 +2552,7 @@
           <t>Vancouver</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2606,6 +2637,7 @@
           <t>Vancouver</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2690,6 +2722,7 @@
           <t>Vancouver</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2774,6 +2807,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2860,6 +2894,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2944,6 +2979,7 @@
           <t>Winnepeg</t>
         </is>
       </c>
+      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3030,6 +3066,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3116,6 +3153,7 @@
           <t>Kingston</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3200,6 +3238,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3284,6 +3323,7 @@
           <t>Vaughan</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3368,6 +3408,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3448,6 +3489,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3532,6 +3574,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3616,6 +3659,7 @@
           <t>Oshawa</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3700,6 +3744,7 @@
           <t>Vaughan</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3786,6 +3831,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3867,6 +3913,7 @@
           <t>Calgary</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3948,6 +3995,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4032,6 +4080,7 @@
           <t>Mississauga</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4108,6 +4157,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4194,6 +4244,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4270,6 +4321,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4350,6 +4402,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4436,6 +4489,7 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4520,6 +4574,307 @@
           <t>Toronto</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>November 20, 2024</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Cover Letter - Fred Li.pdf</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+**EDUCATION**
+Washington University in St. Louis (WashU)	St. Louis, MO, USA
+M.S. in Finance, Quantitative	Sep 2023 - Dec 2024
+- GPA: 3.95/4.00, Rank 2/89
+- Honors: All-semester Dean's List, Beta Gamma Sigma Award, Charles F. Knight Scholar (Expected)
+- Coursework: Continuous-Time Finance (Ph.D. Level), Stochastic Calculus, Exotic &amp; Fixed Income Derivative Pricing, SQL and Database Design, Python &amp; R Machine Learning, LASSO, Quantitative Risk Management, Advanced Corporate Finance I &amp; II
+The University of Hong Kong (HKU)	Hong Kong
+B.S. in Economics and Finance	Sep 2017 - May 2021
+- Rank top 35%, Graduated with 2:1 Distinction, Selected as C.V. Starr Scholarship recipient to exchange at Sciences Po Paris
+**PROFESSIONAL EXPERIENCE**
+Olin Business School at Washington University in St. Louis	St. Louis, MO, USA
+Research Intern	May 2024 - Present
+- Selected Project: Python-driven, Real-time Political Speech Sentiment Signal Tool on Abnormal Market Movements
+    o	Developed a Selenium Chrome-driver scraper to extract U.S. congressional hearing scripts and related social media accounts
+    o	Fine-tuned BERT Topic Model and its sub-models to implement topic classification of the congressional hearing database
+    o	Built an anomaly detection model on sentiment trends to flag moments where sentiment sharply deviates from baseline
+    o	Created an automated alert mechanism triggered by specific keywords, phrases, or sentiment shifts against fiscal and monetary policies, to enable rapid responses to market-moving and short-term trading opportunities
+- Overlaid UK budget announcement shock with market data to visualize how certain political event statements or sentiment trends coincide with market price changes, supporting research project on fiscal shock omitted variable bias (OVB)
+Privium Fund Management	Hong Kong
+Portfolio Manager - US$ 200M Option Selling (Short Straddle) Strategy	Apr 2022 - Dec 2022
+- Co-managed the strategy, applied Black-Scholes and Heston-Nandi GARCH option pricing to optimize premium income
+- Ensured macro-overlay and market breadth, evaluated liquidity and volatility metrics to align trades with market trends
+- Applied pricing models (Heston, Barra, Black-Litterman, Greek hedging) for underlying asset price prediction and risk alignment
+- Controlled portfolio risk through diversification to mitigate contagion and application of risk models to evaluate potential losses
+- Optimized strategies, utilized algorithmic trading to minimize slippage, enhance efficiency, and reduce risk exposure
+- Integrated transaction costs, stress testing, and market impact analysis to guarantee accurate performance metrics
+Yong Rong Asset	Hong Kong
+Junior Trader - US$ 30M High Conviction Sub-fund	Jun 2021 - Jan 2022
+- Analyzed and constructed trade flows, submitting orders and collaborating with counterparties to optimize trading outcomes
+- Utilized strategies such as limit orders, VWAP, TWAP to achieve optimal execution and transaction cost control (TCA)
+- Supported strategic asset allocation, used VBA to streamline trading script maintenance and Net Asset Value report process
+Peak Global Investments	Hong Kong
+Private Equity Intern	Sep 2020 - May 2021
+- Researched cryptocurrency exchanges across Asia and Europe, liaised with senior executives to prepare for acquisitions
+- Assessed client pain points and formulated pitch decks for management team in business development presentations
+- Collaborated with world's largest crypto exchange, applied API to assess targets' trading volumes and their authenticity
+**PROJECT EXPERIENCE**
+Microstructure-Informed End-of-Day Frequency Trading Strategy	St. Louis, MO, USA
+Trading Strategy Design	Oct 2024 - Present
+- Currently developing a proprietary end-of-day (EoD) frequency trading strategy, leveraging market microstructure analysis and machine learning techniques (LASSO, LSTM, kNN) to predict price movements and execute trades in the U.S. equities market
+Hull-White Model Calibration for At-the-Money (ATM) Caplets and Caps	St. Louis, MO, USA
+Outputs: fredhli.github.io/projects/#hull-white-model-calibration  	Mar 2024 - May 2024
+- Implemented closed-form caplet pricing solutions and Monte-Carlo price check, to optimize Hull-White model parameters against ATM Caplet market data, achieving high accuracy in long-maturity cap pricing &gt; 15 years with less than 3% function value loss
+**SKILLS AND QUALIFICATIONS**
+Certificates 	  CFA Level I, HKSFC Type 4 &amp; 9: Advise on Securities &amp; Asset Management License
+Teaching	  TA for: Options, Futures and Derivative Securities (Undergraduate); Behavioral Finance (Graduate)
+Research	  RA for: Research on PEVC-backed companies - under Prof. Minmo Gahng, Cornell University
+Volunteering	  NGO Marketing Director, Soap Cycling HKU; Village School Teacher, Beyond the Pivot HKU
+Programming	  Proficient in Python, R, SQL, Git, VBA, LaTeX; Intermediate in Stata, MATLAB; Basic in JavaScript
+Work Permits	  Hong Kong SAR (Permanent Citizenship), Canada (OWP with Citizenship Assurance), USA (OPT)
+</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+About the job
+Job Summary
+Job Description
+What is the opportunity?
+The Derivative Valuation Analyst is responsible for the timely and accurate analysis, valuation, validation and reconciliation of Listed, OTC (Over the Counter) Bilateral and OTC Cleared Derivatives, as well as of alternative investment products, impacting key lines of business including fund services, pension reporting, insurance reporting, custody reporting and all value added services.
+Please note, this position may cover a late and/or rotating shift schedule.
+What will you do?
+Perform the daily
+Routine tasks such as setup of Listed Derivatives and OTC Derivatives, in Valuation systems
+Tasks for listed Derivatives pricing and analyzing price movements
+OTC/alternative instruments valuation and measure impact of the daily changes in market data inputs to value of the instrument
+Reconciliation against third party statements
+Act as the main liaison with Investment Managers and the internal Trades processing team on new deals and supports the communication of deal price variances that exceed tolerances to the Investment Managers and obtain confirmation
+Participate in research of appropriate valuation methodology for new complex OTC products traded by clients
+Participate in the execution around key project deliverables and identify opportunities to stream line processes and increase productivity
+Ensure compliance with all policies, procedures and standards for all aspects of the business as defined through Risk, Compliance, Operational reviews and audits
+Cover early/late shifts to support the business within global operating model
+What do you need to succeed?
+Must-have:
+Undergraduate Degree in Finance, Math or Engineering
+2+ years of solid experience with Derivatives in a middle or back office environment
+Experience with OTC Derivatives valuation systems and Workflows
+Strong understanding of Reuters, Bloomberg and other financial data providers
+Strong PC skills (advanced proficiency in MS Excel, some knowledge of basic coding such as VBA)
+What's in it for you?
+We thrive on the challenge to be our best, progressive thinking to keep growing, and working together to deliver trusted advice to help our clients thrive and communities prosper. We care about each other, reaching our potential, making a difference to our communities, and achieving success that is mutual.
+Excellent exposure to communicate with various business partners and stakeholders in Investor Services and within other platforms as appropriate
+Opportunity to obtain hands-on experience throughout your role
+Working with an exciting, close-knit, supportive &amp; dynamic group
+Opportunity to collaborate with other business segments within the bank
+Excellent career development and progression opportunities
+A comprehensive Total Rewards Program including bonuses and flexible benefits
+Competitive compensation
+Job Skills
+Active Learning, Adaptability, Business Appraisals, Critical Thinking, Customer Service, Decision Making, Effectiveness Measurement, Operational Delivery, Process Improvements
+Additional Job Details
+Address:
+RBC CENTRE, 155 WELLINGTON ST W:TORONTO
+City:
+TORONTO
+Country:
+Canada
+Work hours/week:
+37.5
+Employment Type:
+Full time
+Platform:
+WEALTH MANAGEMENT
+Job Type:
+Regular
+Pay Type:
+Salaried
+Posted Date:
+2024-10-17
+Application Deadline:
+2024-11-27
+Note: Applications will be accepted until 11:59 PM on the day prior to the application deadline date above
+Inclusion and Equal Opportunity Employment
+At RBC, we embrace diversity and inclusion for innovation and growth. We are committed to building inclusive teams and an equitable workplace for our employees to bring their true selves to work. We are taking actions to tackle issues of inequity and systemic bias to support our diverse talent, clients and communities.
+We also strive to provide an accessible candidate experience for our prospective employees with different abilities. Please let us know if you need any accommodations during the recruitment process.
+Join our Talent Community
+Stay in-the-know about great career opportunities at RBC. Sign up and get customized info on our latest jobs, career tips and Recruitment events that matter to you.
+Expand your limits and create a new future together at RBC. Find out how we use our passion and drive to enhance the well-being of our clients and communities
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>November 20, 2024</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>With Derivative Valuation Analyst</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Cover Letter - Fred Li.pdf</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+**EDUCATION**
+Washington University in St. Louis (WashU)	St. Louis, MO, USA
+M.S. in Finance, Quantitative	Sep 2023 - Dec 2024
+- GPA: 3.95/4.00, Rank 2/89
+- Honors: All-semester Dean's List, Beta Gamma Sigma Award, Charles F. Knight Scholar (Expected)
+- Coursework: Continuous-Time Finance (Ph.D. Level), Stochastic Calculus, Exotic &amp; Fixed Income Derivative Pricing, SQL and Database Design, Python &amp; R Machine Learning, LASSO, Quantitative Risk Management, Advanced Corporate Finance I &amp; II
+The University of Hong Kong (HKU)	Hong Kong
+B.S. in Economics and Finance	Sep 2017 - May 2021
+- Rank top 35%, Graduated with 2:1 Distinction, Selected as C.V. Starr Scholarship recipient to exchange at Sciences Po Paris
+**PROFESSIONAL EXPERIENCE**
+Olin Business School at Washington University in St. Louis	St. Louis, MO, USA
+Research Intern	May 2024 - Present
+- Selected Project: Python-driven, Real-time Political Speech Sentiment Signal Tool on Abnormal Market Movements
+    o	Developed a Selenium Chrome-driver scraper to extract U.S. congressional hearing scripts and related social media accounts
+    o	Fine-tuned BERT Topic Model and its sub-models to implement topic classification of the congressional hearing database
+    o	Built an anomaly detection model on sentiment trends to flag moments where sentiment sharply deviates from baseline
+    o	Created an automated alert mechanism triggered by specific keywords, phrases, or sentiment shifts against fiscal and monetary policies, to enable rapid responses to market-moving and short-term trading opportunities
+- Overlaid UK budget announcement shock with market data to visualize how certain political event statements or sentiment trends coincide with market price changes, supporting research project on fiscal shock omitted variable bias (OVB)
+Privium Fund Management	Hong Kong
+Portfolio Manager - US$ 200M Option Selling (Short Straddle) Strategy	Apr 2022 - Dec 2022
+- Co-managed the strategy, applied Black-Scholes and Heston-Nandi GARCH option pricing to optimize premium income
+- Ensured macro-overlay and market breadth, evaluated liquidity and volatility metrics to align trades with market trends
+- Applied pricing models (Heston, Barra, Black-Litterman, Greek hedging) for underlying asset price prediction and risk alignment
+- Controlled portfolio risk through diversification to mitigate contagion and application of risk models to evaluate potential losses
+- Optimized strategies, utilized algorithmic trading to minimize slippage, enhance efficiency, and reduce risk exposure
+- Integrated transaction costs, stress testing, and market impact analysis to guarantee accurate performance metrics
+Yong Rong Asset	Hong Kong
+Junior Trader - US$ 30M High Conviction Sub-fund	Jun 2021 - Jan 2022
+- Analyzed and constructed trade flows, submitting orders and collaborating with counterparties to optimize trading outcomes
+- Utilized strategies such as limit orders, VWAP, TWAP to achieve optimal execution and transaction cost control (TCA)
+- Supported strategic asset allocation, used VBA to streamline trading script maintenance and Net Asset Value report process
+Peak Global Investments	Hong Kong
+Private Equity Intern	Sep 2020 - May 2021
+- Researched cryptocurrency exchanges across Asia and Europe, liaised with senior executives to prepare for acquisitions
+- Assessed client pain points and formulated pitch decks for management team in business development presentations
+- Collaborated with world's largest crypto exchange, applied API to assess targets' trading volumes and their authenticity
+**PROJECT EXPERIENCE**
+Microstructure-Informed End-of-Day Frequency Trading Strategy	St. Louis, MO, USA
+Trading Strategy Design	Oct 2024 - Present
+- Currently developing a proprietary end-of-day (EoD) frequency trading strategy, leveraging market microstructure analysis and machine learning techniques (LASSO, LSTM, kNN) to predict price movements and execute trades in the U.S. equities market
+Hull-White Model Calibration for At-the-Money (ATM) Caplets and Caps	St. Louis, MO, USA
+Outputs: fredhli.github.io/projects/#hull-white-model-calibration  	Mar 2024 - May 2024
+- Implemented closed-form caplet pricing solutions and Monte-Carlo price check, to optimize Hull-White model parameters against ATM Caplet market data, achieving high accuracy in long-maturity cap pricing &gt; 15 years with less than 3% function value loss
+**SKILLS AND QUALIFICATIONS**
+Certificates 	  CFA Level I, HKSFC Type 4 &amp; 9: Advise on Securities &amp; Asset Management License
+Teaching	  TA for: Options, Futures and Derivative Securities (Undergraduate); Behavioral Finance (Graduate)
+Research	  RA for: Research on PEVC-backed companies - under Prof. Minmo Gahng, Cornell University
+Volunteering	  NGO Marketing Director, Soap Cycling HKU; Village School Teacher, Beyond the Pivot HKU
+Programming	  Proficient in Python, R, SQL, Git, VBA, LaTeX; Intermediate in Stata, MATLAB; Basic in JavaScript
+Work Permits	  Hong Kong SAR (Permanent Citizenship), Canada (OWP with Citizenship Assurance), USA (OPT)
+</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+About the job
+Job Summary
+Job Description
+What is the opportunity?
+The Derivative Valuation Analyst is responsible for the timely and accurate analysis, valuation, validation and reconciliation of Listed, OTC (Over the Counter) Bilateral and OTC Cleared Derivatives, as well as of alternative investment products, impacting key lines of business including fund services, pension reporting, insurance reporting, custody reporting and all value added services.
+Please note, this position may cover a late and/or rotating shift schedule.
+What will you do?
+Perform the daily
+Routine tasks such as setup of Listed Derivatives and OTC Derivatives, in Valuation systems
+Tasks for listed Derivatives pricing and analyzing price movements
+OTC/alternative instruments valuation and measure impact of the daily changes in market data inputs to value of the instrument
+Reconciliation against third party statements
+Act as the main liaison with Investment Managers and the internal Trades processing team on new deals and supports the communication of deal price variances that exceed tolerances to the Investment Managers and obtain confirmation
+Participate in research of appropriate valuation methodology for new complex OTC products traded by clients
+Participate in the execution around key project deliverables and identify opportunities to stream line processes and increase productivity
+Ensure compliance with all policies, procedures and standards for all aspects of the business as defined through Risk, Compliance, Operational reviews and audits
+Cover early/late shifts to support the business within global operating model
+What do you need to succeed?
+Must-have:
+Undergraduate Degree in Finance, Math or Engineering
+2+ years of solid experience with Derivatives in a middle or back office environment
+Experience with OTC Derivatives valuation systems and Workflows
+Strong understanding of Reuters, Bloomberg and other financial data providers
+Strong PC skills (advanced proficiency in MS Excel, some knowledge of basic coding such as VBA)
+What's in it for you?
+We thrive on the challenge to be our best, progressive thinking to keep growing, and working together to deliver trusted advice to help our clients thrive and communities prosper. We care about each other, reaching our potential, making a difference to our communities, and achieving success that is mutual.
+Excellent exposure to communicate with various business partners and stakeholders in Investor Services and within other platforms as appropriate
+Opportunity to obtain hands-on experience throughout your role
+Working with an exciting, close-knit, supportive &amp; dynamic group
+Opportunity to collaborate with other business segments within the bank
+Excellent career development and progression opportunities
+A comprehensive Total Rewards Program including bonuses and flexible benefits
+Competitive compensation
+Job Skills
+Active Learning, Adaptability, Business Appraisals, Critical Thinking, Customer Service, Decision Making, Effectiveness Measurement, Operational Delivery, Process Improvements
+Additional Job Details
+Address:
+RBC CENTRE, 155 WELLINGTON ST W:TORONTO
+City:
+TORONTO
+Country:
+Canada
+Work hours/week:
+37.5
+Employment Type:
+Full time
+Platform:
+WEALTH MANAGEMENT
+Job Type:
+Regular
+Pay Type:
+Salaried
+Posted Date:
+2024-10-17
+Application Deadline:
+2024-11-27
+Note: Applications will be accepted until 11:59 PM on the day prior to the application deadline date above
+Inclusion and Equal Opportunity Employment
+At RBC, we embrace diversity and inclusion for innovation and growth. We are committed to building inclusive teams and an equitable workplace for our employees to bring their true selves to work. We are taking actions to tackle issues of inequity and systemic bias to support our diverse talent, clients and communities.
+We also strive to provide an accessible candidate experience for our prospective employees with different abilities. Please let us know if you need any accommodations during the recruitment process.
+Join our Talent Community
+Stay in-the-know about great career opportunities at RBC. Sign up and get customized info on our latest jobs, career tips and Recruitment events that matter to you.
+Expand your limits and create a new future together at RBC. Find out how we use our passion and drive to enhance the well-being of our clients and communities
+</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor text parsing in notion_functions.py to split by paragraphs, improve formatting logic, and enhance cover letter prompt clarity in gpt_functions.py.
</commit_message>
<xml_diff>
--- a/Application History.xlsx
+++ b/Application History.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4876,6 +4876,158 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>November 20, 2024</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>**Derivative Valuation Analyst**</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Cover Letter - Fred Li.pdf</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+**EDUCATION**
+Washington University in St. Louis (WashU)	St. Louis, MO, USA
+M.S. in Finance, Quantitative	Sep 2023 - Dec 2024
+- GPA: 3.95/4.00, Rank 2/89
+- Honors: All-semester Dean's List, Beta Gamma Sigma Award, Charles F. Knight Scholar (Expected)
+- Coursework: Continuous-Time Finance (Ph.D. Level), Stochastic Calculus, Exotic &amp; Fixed Income Derivative Pricing, SQL and Database Design, Python &amp; R Machine Learning, LASSO, Quantitative Risk Management, Advanced Corporate Finance I &amp; II
+The University of Hong Kong (HKU)	Hong Kong
+B.S. in Economics and Finance	Sep 2017 - May 2021
+- Rank top 35%, Graduated with 2:1 Distinction, Selected as C.V. Starr Scholarship recipient to exchange at Sciences Po Paris
+**PROFESSIONAL EXPERIENCE**
+Olin Business School at Washington University in St. Louis	St. Louis, MO, USA
+Research Intern	May 2024 - Present
+- Selected Project: Python-driven, Real-time Political Speech Sentiment Signal Tool on Abnormal Market Movements
+    o	Developed a Selenium Chrome-driver scraper to extract U.S. congressional hearing scripts and related social media accounts
+    o	Fine-tuned BERT Topic Model and its sub-models to implement topic classification of the congressional hearing database
+    o	Built an anomaly detection model on sentiment trends to flag moments where sentiment sharply deviates from baseline
+    o	Created an automated alert mechanism triggered by specific keywords, phrases, or sentiment shifts against fiscal and monetary policies, to enable rapid responses to market-moving and short-term trading opportunities
+- Overlaid UK budget announcement shock with market data to visualize how certain political event statements or sentiment trends coincide with market price changes, supporting research project on fiscal shock omitted variable bias (OVB)
+Privium Fund Management	Hong Kong
+Portfolio Manager - US$ 200M Option Selling (Short Straddle) Strategy	Apr 2022 - Dec 2022
+- Co-managed the strategy, applied Black-Scholes and Heston-Nandi GARCH option pricing to optimize premium income
+- Ensured macro-overlay and market breadth, evaluated liquidity and volatility metrics to align trades with market trends
+- Applied pricing models (Heston, Barra, Black-Litterman, Greek hedging) for underlying asset price prediction and risk alignment
+- Controlled portfolio risk through diversification to mitigate contagion and application of risk models to evaluate potential losses
+- Optimized strategies, utilized algorithmic trading to minimize slippage, enhance efficiency, and reduce risk exposure
+- Integrated transaction costs, stress testing, and market impact analysis to guarantee accurate performance metrics
+Yong Rong Asset	Hong Kong
+Junior Trader - US$ 30M High Conviction Sub-fund	Jun 2021 - Jan 2022
+- Analyzed and constructed trade flows, submitting orders and collaborating with counterparties to optimize trading outcomes
+- Utilized strategies such as limit orders, VWAP, TWAP to achieve optimal execution and transaction cost control (TCA)
+- Supported strategic asset allocation, used VBA to streamline trading script maintenance and Net Asset Value report process
+Peak Global Investments	Hong Kong
+Private Equity Intern	Sep 2020 - May 2021
+- Researched cryptocurrency exchanges across Asia and Europe, liaised with senior executives to prepare for acquisitions
+- Assessed client pain points and formulated pitch decks for management team in business development presentations
+- Collaborated with world's largest crypto exchange, applied API to assess targets' trading volumes and their authenticity
+**PROJECT EXPERIENCE**
+Microstructure-Informed End-of-Day Frequency Trading Strategy	St. Louis, MO, USA
+Trading Strategy Design	Oct 2024 - Present
+- Currently developing a proprietary end-of-day (EoD) frequency trading strategy, leveraging market microstructure analysis and machine learning techniques (LASSO, LSTM, kNN) to predict price movements and execute trades in the U.S. equities market
+Hull-White Model Calibration for At-the-Money (ATM) Caplets and Caps	St. Louis, MO, USA
+Outputs: fredhli.github.io/projects/#hull-white-model-calibration  	Mar 2024 - May 2024
+- Implemented closed-form caplet pricing solutions and Monte-Carlo price check, to optimize Hull-White model parameters against ATM Caplet market data, achieving high accuracy in long-maturity cap pricing &gt; 15 years with less than 3% function value loss
+**SKILLS AND QUALIFICATIONS**
+Certificates 	  CFA Level I, HKSFC Type 4 &amp; 9: Advise on Securities &amp; Asset Management License
+Teaching	  TA for: Options, Futures and Derivative Securities (Undergraduate); Behavioral Finance (Graduate)
+Research	  RA for: Research on PEVC-backed companies - under Prof. Minmo Gahng, Cornell University
+Volunteering	  NGO Marketing Director, Soap Cycling HKU; Village School Teacher, Beyond the Pivot HKU
+Programming	  Proficient in Python, R, SQL, Git, VBA, LaTeX; Intermediate in Stata, MATLAB; Basic in JavaScript
+Work Permits	  Hong Kong SAR (Permanent Citizenship), Canada (OWP with Citizenship Assurance), USA (OPT)
+</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+About the job
+Job Summary
+Job Description
+What is the opportunity?
+The Derivative Valuation Analyst is responsible for the timely and accurate analysis, valuation, validation and reconciliation of Listed, OTC (Over the Counter) Bilateral and OTC Cleared Derivatives, as well as of alternative investment products, impacting key lines of business including fund services, pension reporting, insurance reporting, custody reporting and all value added services.
+Please note, this position may cover a late and/or rotating shift schedule.
+What will you do?
+Perform the daily
+Routine tasks such as setup of Listed Derivatives and OTC Derivatives, in Valuation systems
+Tasks for listed Derivatives pricing and analyzing price movements
+OTC/alternative instruments valuation and measure impact of the daily changes in market data inputs to value of the instrument
+Reconciliation against third party statements
+Act as the main liaison with Investment Managers and the internal Trades processing team on new deals and supports the communication of deal price variances that exceed tolerances to the Investment Managers and obtain confirmation
+Participate in research of appropriate valuation methodology for new complex OTC products traded by clients
+Participate in the execution around key project deliverables and identify opportunities to stream line processes and increase productivity
+Ensure compliance with all policies, procedures and standards for all aspects of the business as defined through Risk, Compliance, Operational reviews and audits
+Cover early/late shifts to support the business within global operating model
+What do you need to succeed?
+Must-have:
+Undergraduate Degree in Finance, Math or Engineering
+2+ years of solid experience with Derivatives in a middle or back office environment
+Experience with OTC Derivatives valuation systems and Workflows
+Strong understanding of Reuters, Bloomberg and other financial data providers
+Strong PC skills (advanced proficiency in MS Excel, some knowledge of basic coding such as VBA)
+What's in it for you?
+We thrive on the challenge to be our best, progressive thinking to keep growing, and working together to deliver trusted advice to help our clients thrive and communities prosper. We care about each other, reaching our potential, making a difference to our communities, and achieving success that is mutual.
+Excellent exposure to communicate with various business partners and stakeholders in Investor Services and within other platforms as appropriate
+Opportunity to obtain hands-on experience throughout your role
+Working with an exciting, close-knit, supportive &amp; dynamic group
+Opportunity to collaborate with other business segments within the bank
+Excellent career development and progression opportunities
+A comprehensive Total Rewards Program including bonuses and flexible benefits
+Competitive compensation
+Job Skills
+Active Learning, Adaptability, Business Appraisals, Critical Thinking, Customer Service, Decision Making, Effectiveness Measurement, Operational Delivery, Process Improvements
+Additional Job Details
+Address:
+RBC CENTRE, 155 WELLINGTON ST W:TORONTO
+City:
+TORONTO
+Country:
+Canada
+Work hours/week:
+37.5
+Employment Type:
+Full time
+Platform:
+WEALTH MANAGEMENT
+Job Type:
+Regular
+Pay Type:
+Salaried
+Posted Date:
+2024-10-17
+Application Deadline:
+2024-11-27
+Note: Applications will be accepted until 11:59 PM on the day prior to the application deadline date above
+Inclusion and Equal Opportunity Employment
+At RBC, we embrace diversity and inclusion for innovation and growth. We are committed to building inclusive teams and an equitable workplace for our employees to bring their true selves to work. We are taking actions to tackle issues of inequity and systemic bias to support our diverse talent, clients and communities.
+We also strive to provide an accessible candidate experience for our prospective employees with different abilities. Please let us know if you need any accommodations during the recruitment process.
+Join our Talent Community
+Stay in-the-know about great career opportunities at RBC. Sign up and get customized info on our latest jobs, career tips and Recruitment events that matter to you.
+Expand your limits and create a new future together at RBC. Find out how we use our passion and drive to enhance the well-being of our clients and communities
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove cv_info.py and refactor related functions in notion_functions.py and gpt_functions.py to improve code organization and maintainability.
</commit_message>
<xml_diff>
--- a/Application History.xlsx
+++ b/Application History.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5028,6 +5028,158 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>November 20, 2024</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Derivative Valuation Analyst</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Cover Letter - Fred Li.pdf</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+**EDUCATION**
+Washington University in St. Louis (WashU)	St. Louis, MO, USA
+M.S. in Finance, Quantitative	Sep 2023 - Dec 2024
+- GPA: 3.95/4.00, Rank 2/89
+- Honors: All-semester Dean's List, Beta Gamma Sigma Award, Charles F. Knight Scholar (Expected)
+- Coursework: Continuous-Time Finance (Ph.D. Level), Stochastic Calculus, Exotic &amp; Fixed Income Derivative Pricing, SQL and Database Design, Python &amp; R Machine Learning, LASSO, Quantitative Risk Management, Advanced Corporate Finance I &amp; II
+The University of Hong Kong (HKU)	Hong Kong
+B.S. in Economics and Finance	Sep 2017 - May 2021
+- Rank top 35%, Graduated with 2:1 Distinction, Selected as C.V. Starr Scholarship recipient to exchange at Sciences Po Paris
+**PROFESSIONAL EXPERIENCE**
+Olin Business School at Washington University in St. Louis	St. Louis, MO, USA
+Research Intern	May 2024 - Present
+- Selected Project: Python-driven, Real-time Political Speech Sentiment Signal Tool on Abnormal Market Movements
+    o	Developed a Selenium Chrome-driver scraper to extract U.S. congressional hearing scripts and related social media accounts
+    o	Fine-tuned BERT Topic Model and its sub-models to implement topic classification of the congressional hearing database
+    o	Built an anomaly detection model on sentiment trends to flag moments where sentiment sharply deviates from baseline
+    o	Created an automated alert mechanism triggered by specific keywords, phrases, or sentiment shifts against fiscal and monetary policies, to enable rapid responses to market-moving and short-term trading opportunities
+- Overlaid UK budget announcement shock with market data to visualize how certain political event statements or sentiment trends coincide with market price changes, supporting research project on fiscal shock omitted variable bias (OVB)
+Privium Fund Management	Hong Kong
+Portfolio Manager - US$ 200M Option Selling (Short Straddle) Strategy	Apr 2022 - Dec 2022
+- Co-managed the strategy, applied Black-Scholes and Heston-Nandi GARCH option pricing to optimize premium income
+- Ensured macro-overlay and market breadth, evaluated liquidity and volatility metrics to align trades with market trends
+- Applied pricing models (Heston, Barra, Black-Litterman, Greek hedging) for underlying asset price prediction and risk alignment
+- Controlled portfolio risk through diversification to mitigate contagion and application of risk models to evaluate potential losses
+- Optimized strategies, utilized algorithmic trading to minimize slippage, enhance efficiency, and reduce risk exposure
+- Integrated transaction costs, stress testing, and market impact analysis to guarantee accurate performance metrics
+Yong Rong Asset	Hong Kong
+Junior Trader - US$ 30M High Conviction Sub-fund	Jun 2021 - Jan 2022
+- Analyzed and constructed trade flows, submitting orders and collaborating with counterparties to optimize trading outcomes
+- Utilized strategies such as limit orders, VWAP, TWAP to achieve optimal execution and transaction cost control (TCA)
+- Supported strategic asset allocation, used VBA to streamline trading script maintenance and Net Asset Value report process
+Peak Global Investments	Hong Kong
+Private Equity Intern	Sep 2020 - May 2021
+- Researched cryptocurrency exchanges across Asia and Europe, liaised with senior executives to prepare for acquisitions
+- Assessed client pain points and formulated pitch decks for management team in business development presentations
+- Collaborated with world's largest crypto exchange, applied API to assess targets' trading volumes and their authenticity
+**PROJECT EXPERIENCE**
+Microstructure-Informed End-of-Day Frequency Trading Strategy	St. Louis, MO, USA
+Trading Strategy Design	Oct 2024 - Present
+- Currently developing a proprietary end-of-day (EoD) frequency trading strategy, leveraging market microstructure analysis and machine learning techniques (LASSO, LSTM, kNN) to predict price movements and execute trades in the U.S. equities market
+Hull-White Model Calibration for At-the-Money (ATM) Caplets and Caps	St. Louis, MO, USA
+Outputs: fredhli.github.io/projects/#hull-white-model-calibration  	Mar 2024 - May 2024
+- Implemented closed-form caplet pricing solutions and Monte-Carlo price check, to optimize Hull-White model parameters against ATM Caplet market data, achieving high accuracy in long-maturity cap pricing &gt; 15 years with less than 3% function value loss
+**SKILLS AND QUALIFICATIONS**
+Certificates 	  CFA Level I, HKSFC Type 4 &amp; 9: Advise on Securities &amp; Asset Management License
+Teaching	  TA for: Options, Futures and Derivative Securities (Undergraduate); Behavioral Finance (Graduate)
+Research	  RA for: Research on PEVC-backed companies - under Prof. Minmo Gahng, Cornell University
+Volunteering	  NGO Marketing Director, Soap Cycling HKU; Village School Teacher, Beyond the Pivot HKU
+Programming	  Proficient in Python, R, SQL, Git, VBA, LaTeX; Intermediate in Stata, MATLAB; Basic in JavaScript
+Work Permits	  Hong Kong SAR (Permanent Citizenship), Canada (OWP with Citizenship Assurance), USA (OPT)
+</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+About the job
+Job Summary
+Job Description
+What is the opportunity?
+The Derivative Valuation Analyst is responsible for the timely and accurate analysis, valuation, validation and reconciliation of Listed, OTC (Over the Counter) Bilateral and OTC Cleared Derivatives, as well as of alternative investment products, impacting key lines of business including fund services, pension reporting, insurance reporting, custody reporting and all value added services.
+Please note, this position may cover a late and/or rotating shift schedule.
+What will you do?
+Perform the daily
+Routine tasks such as setup of Listed Derivatives and OTC Derivatives, in Valuation systems
+Tasks for listed Derivatives pricing and analyzing price movements
+OTC/alternative instruments valuation and measure impact of the daily changes in market data inputs to value of the instrument
+Reconciliation against third party statements
+Act as the main liaison with Investment Managers and the internal Trades processing team on new deals and supports the communication of deal price variances that exceed tolerances to the Investment Managers and obtain confirmation
+Participate in research of appropriate valuation methodology for new complex OTC products traded by clients
+Participate in the execution around key project deliverables and identify opportunities to stream line processes and increase productivity
+Ensure compliance with all policies, procedures and standards for all aspects of the business as defined through Risk, Compliance, Operational reviews and audits
+Cover early/late shifts to support the business within global operating model
+What do you need to succeed?
+Must-have:
+Undergraduate Degree in Finance, Math or Engineering
+2+ years of solid experience with Derivatives in a middle or back office environment
+Experience with OTC Derivatives valuation systems and Workflows
+Strong understanding of Reuters, Bloomberg and other financial data providers
+Strong PC skills (advanced proficiency in MS Excel, some knowledge of basic coding such as VBA)
+What's in it for you?
+We thrive on the challenge to be our best, progressive thinking to keep growing, and working together to deliver trusted advice to help our clients thrive and communities prosper. We care about each other, reaching our potential, making a difference to our communities, and achieving success that is mutual.
+Excellent exposure to communicate with various business partners and stakeholders in Investor Services and within other platforms as appropriate
+Opportunity to obtain hands-on experience throughout your role
+Working with an exciting, close-knit, supportive &amp; dynamic group
+Opportunity to collaborate with other business segments within the bank
+Excellent career development and progression opportunities
+A comprehensive Total Rewards Program including bonuses and flexible benefits
+Competitive compensation
+Job Skills
+Active Learning, Adaptability, Business Appraisals, Critical Thinking, Customer Service, Decision Making, Effectiveness Measurement, Operational Delivery, Process Improvements
+Additional Job Details
+Address:
+RBC CENTRE, 155 WELLINGTON ST W:TORONTO
+City:
+TORONTO
+Country:
+Canada
+Work hours/week:
+37.5
+Employment Type:
+Full time
+Platform:
+WEALTH MANAGEMENT
+Job Type:
+Regular
+Pay Type:
+Salaried
+Posted Date:
+2024-10-17
+Application Deadline:
+2024-11-27
+Note: Applications will be accepted until 11:59 PM on the day prior to the application deadline date above
+Inclusion and Equal Opportunity Employment
+At RBC, we embrace diversity and inclusion for innovation and growth. We are committed to building inclusive teams and an equitable workplace for our employees to bring their true selves to work. We are taking actions to tackle issues of inequity and systemic bias to support our diverse talent, clients and communities.
+We also strive to provide an accessible candidate experience for our prospective employees with different abilities. Please let us know if you need any accommodations during the recruitment process.
+Join our Talent Community
+Stay in-the-know about great career opportunities at RBC. Sign up and get customized info on our latest jobs, career tips and Recruitment events that matter to you.
+Expand your limits and create a new future together at RBC. Find out how we use our passion and drive to enhance the well-being of our clients and communities
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor gpt_functions.py to use a dynamic model parameter in chatgpt calls for improved flexibility and maintainability.
</commit_message>
<xml_diff>
--- a/Application History.xlsx
+++ b/Application History.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="241">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,15 @@
     <t>February 10, 2025</t>
   </si>
   <si>
+    <t>February 12, 2025</t>
+  </si>
+  <si>
+    <t>February 13, 2025</t>
+  </si>
+  <si>
+    <t>February 17, 2025</t>
+  </si>
+  <si>
     <t>Cumberland Private Wealth</t>
   </si>
   <si>
@@ -277,6 +286,12 @@
     <t>Mastery Trust Limited</t>
   </si>
   <si>
+    <t>Citi</t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
     <t>Internal Auditor</t>
   </si>
   <si>
@@ -494,6 +509,24 @@
   </si>
   <si>
     <t>Research Associate, TMT, Research</t>
+  </si>
+  <si>
+    <t>Assistant Manager (Finance)</t>
+  </si>
+  <si>
+    <t>TRAINEE: Junior Structurer</t>
+  </si>
+  <si>
+    <t>Research Associate - HONG KONG</t>
+  </si>
+  <si>
+    <t>Investment Analyst, Hong Kong</t>
+  </si>
+  <si>
+    <t>Officer, FX Derivatives Settlement Analyst</t>
+  </si>
+  <si>
+    <t>Analyst, Operations</t>
   </si>
   <si>
     <t>Cover Letter - Fred Li.pdf</t>
@@ -2491,6 +2524,288 @@
 High sense of commercial awareness
 Excellent interpersonal sensitivity.  Excellent communication and management skills to both internal and external clients
 Fluent in English and Mandarin is a must, knowledge in Cantonese is an advantage but not essential
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+What is this position about?
+The Finance Implementation Project (FIP) is in charge to drive and deliver the end-to-end regulatory and business projects implementation. The main mission is to integrate in Finance systems business processes and regulatory requirements, in accordance with Norms &amp; Standards, to embrace all streams of Reporting (Financial Accounting, Management Accounting, Credit Risk, Liquidity). The APAC FIP team is part of the global FIP organization who is responsible for all accounting projects in APAC region. 
+Mission statement  
+•    Ensure the end-to-end implementation of the Business and Regulatory projects, in full alignment with Finance strategy.
+•    Respond to the various businesses and reporting requirements (Financial Accounting, Management Accounting, Credit Risk, Liquidity etc.) in a timely manner.
+•    Source and transform raw data and enable a good quality of reporting.
+•    Ensure a consistent approach of the Finance solutions across the region and align to Group standard.
+Role and responsibility 
+•    Lead and drive the ledger transformation project in Finance in the context of ever changing business &amp; regulatory reporting requirements.  
+•    Ensure consistency of Finance systems/reports across the APAC region, in adherence to the Group's standard.  
+•    Provide efficient support to Finance teams in daily production tasks, whenever required
+•    Act as a bridge between request and the delivery of solution
+•    Major projects involve:
+o    Build or automate the accounting interface between operating systems and accounting core ledger systems
+o    Support new business and new products initiatives 
+o    Support new regulatory requirements
+o    System upgrades and migrations
+Our values
+•    We are keen to understand our clients and serve our clients better.
+•    Focus on time-to-market and delivery to address business's needs. 
+•    Emphasize on collaboration between teams to deliver solutions in the bank's best interest. 
+•    We believe there are always solutions. 
+What would be your typical day at BNPP Paribas look like? 
+Primary Role Responsibilities
+•    Acting as a Business Analyst (70%)
+-    Understand the project objective and ensure all user requirements are properly captured
+-    Carry out feasibility study, assess potential impact and define target operating model
+-    Explain the user requirements to IT for IT development
+-    Define the appropriate testing strategy according to the nature of the project
+-    Design test cases and ensure adequate testing is performed
+-    Validate testing result by performing detailed checking of accounting entries and/ or reports and provide UAT sign-off on behalf of finance users
+•    Acting as a Project Manager (30%) 
+-    Drive and manage all stages in project life cycle, from project initialization to project closure
+-    Develop project scope documentation, project plans and project schedules 
+-    Continuously coordinate with IT and other finance users
+-    Undertake risk analysis and proactively identify mitigating solutions
+-    Timely track the progress of projects against agreed timeline and budget 
+-    Arrange smooth go-live implementation and provide post go-live support
+-    Present project status regularly to senior management
+-    Build and maintain a trusted relationship with all project stakeholders across different functions (PMO, IT, finance users, operation teams)
+•    Provide support in case of production incidents, including root cause identification and proposing solutions to resolve the issue in a timely manner
+Other contributions
+•    Identify areas of improvement; streamline the existing processes for efficiency
+•    Support team-head to monitor the budget and share progress updates
+What is required for you to succeed?
+Technical Competencies
+o    Accounting related experience And / Or finance project experience in Financial Institution (5+ years)
+o    CPA preferred, but not mandatory
+o    Experience in project management and PMP qualification preferred, but not necessary
+o    Adequate knowledge on accounting treatment (especially on financial instruments) under IFRS
+o    Knowledge on front-to-back operation and financial products would be an advantage
+o    Proven ability in project delivery
+o    Good command of written and spoken English and Mandarin
+o    PC skill such as MS Word, Excel, PowerPoint, SQL
+Behavioral Competencies
+o    Excited about driving change
+o    Strong communication and interpersonal skills
+o    Ability to work in multicultural environment, as the role needs to deal with different stakeholders across APAC regions
+o    Self-driven and able to work independently
+o    Attention to detail
+o    Able to work under stress
+o    Strong problem solving and logical thinking skill
+o    Ability to multi-task
+o    Team player 
+About BNP PARIBAS
+As the leading European Union bank, and one of the world's largest financial institutions with an uninterrupted presence in the region since 1860, BNP Paribas offers a wide range of financial services for corporate, institutional and private investors spanning corporate and institutional banking, wealth management, asset management and insurance. 
+We passionately embrace diversity and are committed to fostering an inclusive workplace where all employees are valued and encourage applicants of all backgrounds, including diversity of origin, age, gender, sexual orientation, gender identity, religion applicants who may be living with a disability. We have a number of internal employee networks in place to empower our staff to act and challenge the status quo.
+•    BNP Paribas PRIDE is highly active in favour of the LGBTQIA+ community
+•    BNP Paribas MixCity which fosters better representation of women at all levels of the organization
+•    Ability, the mutual aid network for employees with a disability or a disabling or chronic illness
+•    BNP Paribas CulturAll which celebrates diverse backgrounds
+BNP is committed to financing a carbon-neutral economy by 2050. The Group is a founding member of the Net-Zero Banking Alliance and has set up its own Low Carbon Transition Group to support its clients through their energy transitions.
+https://careers.apac.bnpparibas/(Opens in a new tab)
+More information 
+BNP Paribas - Diversity &amp; Inclusion Journey
+BNP Paribas - The Bank Of Green Changes
+Award Obtained
+BNPP has won Top employer Europe award in a 10th consecutive year
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Responsibilities
+Complete market studies and analysis: market trends, competitors watch, regulatory watch
+Assist in answering sales or clients' requests
+Participate to new products and solutions design
+Assist in drafting and reviewing products legal documentation (term sheets, final terms, confirmations…)
+Assist in negotiating agreements with clients (distribution agreements, master agreements…) and service providers
+Participate to new products delivery projects, coordinating with internal departments to obtain approvals and to ensure smooth execution
+Help automating documentation generation process (template creation using internal tools)
+Monitor the activity and produce associated reports
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Responsibilities
+Complete market studies and analysis: market trends, competitors watch, regulatory watch
+Assist in answering sales or clients' requests
+Participate to new products and solutions design
+Assist in drafting and reviewing products legal documentation (term sheets, final terms, confirmations…)
+Assist in negotiating agreements with clients (distribution agreements, master agreements…) and service providers
+Participate to new products delivery projects, coordinating with internal departments to obtain approvals and to ensure smooth execution
+Help automating documentation generation process (template creation using internal tools)
+Monitor the activity and produce associated reports
+Profile required
+Hold a relevant Bachelors or Masters degree in Finance, Financial Mathematics, Computer Science, Business, Law or similar
+Interest in financial markets and structured products
+Strong communication and presentation skills
+Excellent organizational skills
+Highly motivated who can work autonomously
+Flexible and adaptable
+Good team player with ability to drive initiatives cross-departments for a common goal
+Self-motivated, responsible, able to work under pressure and meet tight deadline
+Fluent English is mandatory, Mandarin proficiency is preferred     
+This is a fixed term 12-month Trainee contract with Societe Generale. You will form part of the team on a full time basis. In order to apply for the Trainee position please ensure you have completed your qualification and will be available to work full time for the duration of the Trainee contract.
+Behavioral Skills:
+Client - Understanding and Respect: I listen to clients and colleagues in order to understand and anticipate their needs
+Client - Sales and Marketing Strategy: I contribute to adapt our offer to our clients'/internal partners' needs
+Team Spirit - Synergies: I make cooperation with colleagues in and outside my team a priority
+Innovation - Thinking out of the box/Creativity: I propose new ideas and solutions
+Responsibility - Risk awareness: I am constantly on the lookout for risks
+Commitment - Sustainability: I strive to develop my skills and knowledge
+Business insight
+Our Culture:
+At Societe Generale, we live by our 4 core values of commitment, responsibility, team spirit and innovation. We are engaged and demonstrate consideration for others. We act ethically and with courage. We focus our talent and energy on collective success. We experiment and propose new ideas. This way, we maximize our ability to serve client needs and anticipate market changes. Societe Generale is committed to strengthening bonds with colleagues, communities, and the world in which we live, because relationships are at the heart of how we operate.   Please visit our APAC career website: https://www.societegenerale.asia/en/careers/building-your-career-with/ for more information.
+Diversity, Equity &amp; Inclusion (DE&amp;I):
+Our mission: Recruit, develop, advance, and retain a diverse workforce that is united in our efforts to enhance our competitive position and deliver innovative solutions to our clients.
+Our vision:
+Engaged workforce that is demographically diverse in a way that reflects the communities in which we operate
+Inclusive culture and workplace that recognizes employees' unique needs and utilizes their diverse talents
+Engage our community and marketplace, and position the organization to meet the needs of all its clients
+Check out our DE&amp;I initiatives: https://www.societegenerale.asia/en/careers/diversity-equity-inclusion-dei/
+Department Description:
+Within the Global Markets Division in Hong Kong, you will join our Financial Engineering department which brings together the Equities, Fixed Income &amp; Currencies structuring capabilities with the objective of providing investors with one integrated multi-asset market solutions team. The department capitalizes on an integrated engineering team to deliver cross asset expertise. You will join the Cross-Asset Structuring team in charge of designing and implementing investment solutions for our clients.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The Research Associate is a developing professional role. Deals with most problems independently and has some latitude to solve complex problems. Integrates in-depth specialty area knowledge with a solid understanding of industry standards and practices. Good understanding of how the team and area integrate with others in accomplishing the objectives of the sub function/ job family. Applies analytical thinking and knowledge of data analysis tools and methodologies. Requires attention to detail when making judgments and recommendations based on the analysis of factual information. Typically deals with variable issues with potentially broader business impact. Applies professional judgment when interpreting data and results. Breaks down information in a systematic and communicable manner. Developed communication and diplomacy skills are required in order to exchange potentially complex/sensitive information. Moderate but direct impact through close contact with the businesses' core activities. Quality and timeliness of service provided will affect the effectiveness of own team and other closely related teams.
+Responsibilities:
+Reviews and processes broker votes to be shared and consumed
+Organizes the product management team including creation of presentations, marketing schedules, coordination of the marketing diary, product planning meetings, diary management etc.
+Publishes focus list notes, updating and displaying the new focus list posters etc.
+Contributes to market data and subscriptions management for Equity Research
+Responsible for collation, co-ordination and organization of Road Ahead conference, stock steering meetings
+Assists with year-end scorecard preparation, result analysis, goals and training
+Provides management information including variance analysis, month-end reporting etc.
+Conducts expense management including travel and entertainment pre-approvals, client interaction spend pre-approval e.g. GLG, non-network individuals etc.
+Manages and prepares Committee quality reviews
+Appropriately assess risk when business decisions are made, demonstrating particular consideration for the firm's reputation and safeguarding Citigroup, its clients and assets, by driving compliance with applicable laws, rules and regulations, adhering to Policy, applying sound ethical judgment regarding personal behavior, conduct and business practices, and escalating, managing and reporting control issues with transparency.
+Qualifications:
+MBA and/or CFA preferred
+Existing knowledge of Research or external Investment research division essential
+History of working within tight deadlines and prioritization
+Microsoft systems especially Excel and Word
+Ability to interact and manage at all levels ability to manage large amounts of data ability to use internal Citi systems would be an advantage but is not essential.
+Accuracy and attention to detail
+Secure and maintain applicable licenses
+Education:
+Bachelor's/University degree or equivalent experience
+------------------------------------------------------
+Job Family Group:
+Research
+------------------------------------------------------
+Job Family:
+Research Analysis
+------------------------------------------------------
+Time Type:
+Full time
+------------------------------------------------------
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+At Citi, we get to connect millions of people across hundreds of cities and countries every day. And we've been doing it for more than 200 years. We do this through our unparalleled global network. We provide a broad range of financial services and products to our clients - whether they be consumers, corporations, governments or institutions - to help them meet their biggest opportunities and face the world's toughest challenges.
+Shape your Career with Citi
+Citi Global Wealth (CGW) brings together the full power of Citi to serve the entire continuum of wealth clients, from affluent to ultra-high net worth to family offices. The strategies we create help our clients maintain liquidity while maximizing yields, transact in foreign currency and across borders, and manage fluctuating expenses or cash flow. We are uniquely suited to helping our clients meet their banking needs across regions through our global network.
+Citi Private Bank (CPB) is dedicated to serving the world's wealthiest individuals and their families.  From 52 locations across 20 countries, we offer our services to more than 14,000 ultra-high net worth clients from nearly 100 nations.  Our clients include entrepreneurs, business leaders, executives, their heirs and families, whom we offer customized services to help protect and responsibly grow their wealth.  Our unique approach focuses on fewer, larger and more sophisticated clients with an average net worth above $100 million.
+We're currently looking for a high caliber professional to join our team as Investment Analyst based in Hong Kong.  Being part of our team means that we'll provide you with the resources to meet your unique needs, empower you to make healthy decision and manage your financial well-being to help plan for your future.  For instance:
+Citi provides programs and services for your physical and mental well-being including access to telehealth options, health advocates, confidential counseling and more. Coverage varies by country.
+We believe all parents deserve time to adjust to parenthood and bond with the newest members of their families. That's why in early 2020 we began rolling out our expanded Paid Parental Leave Policy to include Citi employees around the world.
+We empower our employees to manage their financial well-being and help them plan for the future.
+Citi provides access to an array of learning and development resources to help broaden and deepen your skills and knowledge as your career progresses.
+We have a variety of programs that help employees balance their work and life, including generous paid time off packages.
+We offer our employees resources and tools to volunteer in the communities in which they live and work. In 2019, Citi employee volunteers contributed more than 1 million volunteer hours around the world.
+In this role, you're expected to:
+Help support the senior members of the investment team in their delivery of investment solutions to clients.
+Monitor and provide guidance on the markets to internal and external clients, incorporating the views of The Private Bank's Investment Committee.
+Prepare investment policy statements for prospective clients
+Analyze economic trends/activities and advise the effects on the investors' portfolios
+Recommend changes to the investors' holdings after evaluating the economic, financial and market factors and the potential impact on the investors' portfolios.
+Develop relationships and generate ideas with the bankers and clients that will lead to the growth of the asset base
+In support of senior team members, engage clients on investment themes and solutions, and assist in the execute of the investment solutions and trades.
+Attend internal and external meetings to stay current on financial markets, and products and services offered by Citi Private Bank.
+Adhere to a specific prospecting code of conduct, which (1) permits acquiring new private client accounts only by referral or personal contact with an individual seeking to do business and (2) prohibits seminars, mail campaigns, cold calling and any other methods of solicitation.
+Appropriately assess risk when business decisions are made, demonstrating particular consideration for the firm's reputation and safeguarding Citigroup, its clients and assets, by driving compliance with applicable laws, rules and regulations, adhering to Policy, applying sound ethical judgment regarding personal behavior, conduct and business practices, and escalating, managing and reporting control issues with transparency.
+As a successful candidate, you'd ideally have the following skills and exposure:
+Bachelor's/University degree or equivalent experience
+0-2 years relevant experience
+Bachelor's degree with concentration of economics, finance or business administration; Professional experience or related occupation.
+Strong financial background, ability to communicate with co-workers and clients; excellent written and communication skills, able to work without direction, self-motivated
+Working at Citi is far more than just a job. A career with us means joining a family of more than 230,000 dedicated people from around the globe. At Citi, you'll have the opportunity to grow your career, give back to your community and make a real impact.
+Take the next step in your career, apply for this role at Citi today
+https://jobs.citi.com/dei
+-------------------------------------------------
+Job Family Group:
+Private Client Product Services
+-------------------------------------------------
+Job Family:
+Investment Counselor
+------------------------------------------------------
+Time Type:
+------------------------------------------------------
+Citi is an equal opportunity and affirmative action employer.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+At Citi, we get to connect millions of people across hundreds of cities and countries every day.  And we've been doing it for more than 200 years.  We do this through our unparalleled global network.  We provide a broad range of financial services and products to our clients - whether they be consumers, corporations, governments or institutions - to help them meet their biggest opportunities and face the world's toughest challenges.
+Shape your Career with Citi
+Citi's Markets business provides world-class solutions and an unmatched global presence.  We serve corporates, institutional investors and governments from trading floors in almost 80 countries.  The strength of our underwriting, sales and trading and distribution capabilities span asset classes and currencies, providing us with an unmatched ability to meet the needs of our clients.
+We're currently looking for a high caliber professional to join our team as Officer, FX Derivatives Settlement Analyst - Hybrid (Internal Job Title: Securities &amp; Derivatives Analyst 2 - C10) based in Hong Kong.  Being part of our team means that we'll provide you with the resources to meet your unique needs, empower you to make healthy decision and manage your financial well-being to help plan for your future.  For instance:
+Citi provides programs and services for your physical and mental well-being including access to telehealth options, health advocates, confidential counseling and more. Coverage varies by country.
+We believe all parents deserve time to adjust to parenthood and bond with the newest members of their families. That's why in early 2020 we began rolling out our expanded Paid Parental Leave Policy to include Citi employees around the world.
+We empower our employees to manage their financial well-being and help them plan for the future.
+Citi provides access to an array of learning and development resources to help broaden and deepen your skills and knowledge as your career progresses.
+We have a variety of programs that help employees balance their work and life, including generous paid time off packages.
+We offer our employees resources and tools to volunteer in the communities in which they live and work. In 2019, Citi employee volunteers contributed more than 1 million volunteer hours around the world.
+In this role, you're expected to:
+Process securities transactions, provide analytic input for traders and aid in review of derivative products
+Identify and resolve securities and derivative settlement issues, and make process improvement recommendations to leadership
+Analyze moderately complex reports to satisfy management requirements, aid in control activities, and contribute to the launch of product services
+Monitor and suggest solutions to errors to minimize risk to the bank, through an intermediate knowledge of procedural requirements
+Escalate transaction processing issues to the appropriate department and collaborate on a solution
+Design and analyze moderately complex reports, in coordination with standards set by direct leadership
+Assist with control activities, and the launch of new products and services
+Ensure processes adhere to audit and control policies
+Appropriately assess risk when business decisions are made, demonstrating particular consideration for the firm's reputation and safeguarding Citigroup, its clients and assets, by driving compliance with applicable laws, rules and regulations, adhering to Policy, applying sound ethical judgment regarding personal behavior, conduct and business practices, and escalating, managing and reporting control issues with transparency.
+As a successful candidate, you'd ideally have the following skills and exposure:
+1-3 years of relevant experience
+Fundamental understanding of Treasury Products (particularly IRS, FX Options), accounting and regulatory policies
+Proven ability to perform various concurrent activities/projects in a high-risk environment
+Ability to work in a fast-paced environment
+Demonstrated knowledge of macros
+Bachelor's Degree/University degree or equivalent experience in Business, Accounting, or Finance
+Working at Citi is far more than just a job. A career with us means joining a family of more than 230,000 dedicated people from around the globe. At Citi, you'll have the opportunity to grow your career, give back to your community and make a real impact.
+Take the next step in your career, apply for this role at Citi today
+https://jobs.citi.com/dei
+------------------------------------------------------
+Job Family Group:
+Operations - Transaction Services
+------------------------------------------------------
+Job Family:
+Securities and Derivatives Processing
+------------------------------------------------------
+Time Type:
+Full time
+------------------------------------------------------
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Country: Hong Kong
+To work with Senior Manager to control over day-to-day operations ensuring that the Bank's policies, operational guidelines are adhered to by team members, consistent delivery of quality services to clients and optimal utilization of available resources.
+Key Responsibilities
+1. Review Import/Export documents presented against LC terms and input to relevant trade system.
+2. Handle transactions of Discounting/ Forfeiting/ Import &amp; Export Finance/ Factoring.
+3. Ensure transactions meeting service standard and in accordance with procedure manual.
+4. Conduct AML/ Sanction checking of transactions. Report any suspicious activities per policies and guidelines.
+5. Liaise with internal/external stakeholders including cross countries working partners to resolve Trade related issues.
+6. Perform ad hoc duties and projects assigned by Management as well as cross team support as required to Banking Operations.
+Requirements
+1. Bachelor degree in Business Administration, Operation Management, or related disciplines preferred with solid 3-5 year experience in Trade Services.
+2. Good knowledge in ICC UCP &amp; URC and ISBP.
+3. Sound knowledge in operational risk framework and sensitive to identify irregularities.
+4. Exposure in SWIFT Alliance and Banking Systems.
+5. Proficient in both spoken and written English and Chinese (including Putonghua).
+6. Hands-on experience in MS Words &amp; Excel.
 </t>
   </si>
 </sst>
@@ -2849,7 +3164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2883,16 +3198,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2900,16 +3215,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2917,19 +3232,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2937,19 +3252,19 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2957,16 +3272,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F6" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2974,19 +3289,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2994,19 +3309,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3014,19 +3329,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F9" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3034,16 +3349,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3051,16 +3366,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="F11" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3068,19 +3383,19 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="F12" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3088,19 +3403,19 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F13" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3108,19 +3423,19 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3128,19 +3443,19 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F15" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3148,19 +3463,19 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E16" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3168,19 +3483,19 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F17" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3188,19 +3503,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="F18" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3208,19 +3523,19 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E19" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3228,19 +3543,19 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F20" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3248,19 +3563,19 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F21" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3268,19 +3583,19 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3288,19 +3603,19 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3308,19 +3623,19 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E24" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F24" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3328,19 +3643,19 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="F25" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3348,19 +3663,19 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F26" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3368,19 +3683,19 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E27" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F27" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3388,19 +3703,19 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E28" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F28" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3408,19 +3723,19 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E29" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F29" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3428,19 +3743,19 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E30" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F30" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3448,19 +3763,19 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E31" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F31" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3468,19 +3783,19 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E32" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F32" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3488,19 +3803,19 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E33" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F33" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3508,19 +3823,19 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F34" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3528,19 +3843,19 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F35" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3548,19 +3863,19 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3568,19 +3883,19 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E37" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F37" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3588,16 +3903,16 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E38" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F38" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3605,19 +3920,19 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D39" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E39" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F39" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3625,19 +3940,19 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E40" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F40" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3645,19 +3960,19 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F41" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3665,19 +3980,19 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F42" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3685,19 +4000,19 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E43" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F43" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3705,19 +4020,19 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E44" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F44" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3725,19 +4040,19 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E45" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F45" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3745,19 +4060,19 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F46" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3765,19 +4080,19 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E47" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F47" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3785,19 +4100,19 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F48" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3805,16 +4120,16 @@
         <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F49" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3822,19 +4137,19 @@
         <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E50" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F50" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3842,19 +4157,19 @@
         <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3862,19 +4177,19 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D52" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F52" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G52" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3882,22 +4197,22 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E53" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G53" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3905,22 +4220,22 @@
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E54" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F54" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G54" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3928,22 +4243,22 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E55" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G55" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3951,22 +4266,22 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F56" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G56" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3974,22 +4289,22 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F57" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G57" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3997,22 +4312,22 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E58" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F58" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G58" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -4020,22 +4335,22 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D59" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F59" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G59" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -4043,22 +4358,22 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E60" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F60" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G60" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -4066,22 +4381,22 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E61" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F61" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G61" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -4089,22 +4404,22 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E62" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F62" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G62" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -4112,22 +4427,22 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G63" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -4135,22 +4450,22 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F64" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G64" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -4158,22 +4473,22 @@
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D65" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E65" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G65" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -4181,22 +4496,22 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F66" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G66" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -4204,22 +4519,22 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D67" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E67" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F67" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G67" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -4227,22 +4542,22 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E68" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F68" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G68" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -4250,22 +4565,22 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D69" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F69" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G69" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -4273,22 +4588,22 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D70" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F70" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G70" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -4296,22 +4611,22 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D71" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E71" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F71" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G71" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -4319,22 +4634,22 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E72" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F72" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G72" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -4342,22 +4657,22 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E73" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F73" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G73" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -4365,22 +4680,22 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E74" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F74" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G74" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -4388,22 +4703,22 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E75" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F75" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G75" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -4411,22 +4726,22 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E76" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F76" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G76" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -4434,22 +4749,22 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F77" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G77" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -4457,22 +4772,22 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E78" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F78" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G78" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -4480,22 +4795,22 @@
         <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D79" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E79" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F79" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G79" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4503,22 +4818,22 @@
         <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D80" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E80" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F80" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G80" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4526,22 +4841,22 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D81" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E81" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F81" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G81" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4549,22 +4864,22 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D82" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E82" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F82" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G82" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4572,22 +4887,22 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E83" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F83" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G83" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4595,22 +4910,22 @@
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E84" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F84" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G84" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4618,22 +4933,22 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D85" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E85" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F85" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G85" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4641,22 +4956,22 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D86" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E86" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F86" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G86" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4664,22 +4979,22 @@
         <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D87" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E87" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F87" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G87" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4687,22 +5002,206 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C88" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D88" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E88" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F88" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G88" t="s">
-        <v>222</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>65</v>
+      </c>
+      <c r="C89" t="s">
+        <v>165</v>
+      </c>
+      <c r="D89" t="s">
+        <v>171</v>
+      </c>
+      <c r="E89" t="s">
+        <v>187</v>
+      </c>
+      <c r="F89" t="s">
+        <v>200</v>
+      </c>
+      <c r="G89" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" t="s">
+        <v>166</v>
+      </c>
+      <c r="D90" t="s">
+        <v>171</v>
+      </c>
+      <c r="E90" t="s">
+        <v>187</v>
+      </c>
+      <c r="F90" t="s">
+        <v>200</v>
+      </c>
+      <c r="G90" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C91" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" t="s">
+        <v>171</v>
+      </c>
+      <c r="E91" t="s">
+        <v>187</v>
+      </c>
+      <c r="F91" t="s">
+        <v>200</v>
+      </c>
+      <c r="G91" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" t="s">
+        <v>171</v>
+      </c>
+      <c r="E92" t="s">
+        <v>187</v>
+      </c>
+      <c r="F92" t="s">
+        <v>200</v>
+      </c>
+      <c r="G92" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
+        <v>167</v>
+      </c>
+      <c r="D93" t="s">
+        <v>171</v>
+      </c>
+      <c r="E93" t="s">
+        <v>188</v>
+      </c>
+      <c r="F93" t="s">
+        <v>200</v>
+      </c>
+      <c r="G93" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>22</v>
+      </c>
+      <c r="B94" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" t="s">
+        <v>168</v>
+      </c>
+      <c r="D94" t="s">
+        <v>171</v>
+      </c>
+      <c r="E94" t="s">
+        <v>188</v>
+      </c>
+      <c r="F94" t="s">
+        <v>200</v>
+      </c>
+      <c r="G94" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>22</v>
+      </c>
+      <c r="B95" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" t="s">
+        <v>169</v>
+      </c>
+      <c r="D95" t="s">
+        <v>171</v>
+      </c>
+      <c r="E95" t="s">
+        <v>187</v>
+      </c>
+      <c r="F95" t="s">
+        <v>200</v>
+      </c>
+      <c r="G95" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96" t="s">
+        <v>170</v>
+      </c>
+      <c r="D96" t="s">
+        <v>171</v>
+      </c>
+      <c r="E96" t="s">
+        <v>187</v>
+      </c>
+      <c r="F96" t="s">
+        <v>200</v>
+      </c>
+      <c r="G96" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>